<commit_message>
fixed the issues in using FFTT and waiting time in hour, other than in min
</commit_message>
<xml_diff>
--- a/dataset_v1/02_Braess_Paradox/Braess_network_Process_Tutorial.xlsx
+++ b/dataset_v1/02_Braess_Paradox/Braess_network_Process_Tutorial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18016\Documents\GitHub\DTALite\dataset_v1\02_Braess_Paradox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A0780D-DB21-444B-B8F7-4F7C9B76066B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BFA365-C750-49FF-A243-5C64AF833C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2142,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>